<commit_message>
change img and text
</commit_message>
<xml_diff>
--- a/楊于青計畫表.xlsx
+++ b/楊于青計畫表.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>日</t>
   </si>
@@ -39,39 +40,87 @@
     <t>六</t>
   </si>
   <si>
+    <t>關於</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>規劃日程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>實際日程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>八月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>構想</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>草稿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主頁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>九月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>關於</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>購物</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最後</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>排版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>簡報</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>W5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>W1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>八月</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>九月</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>構想</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主頁</t>
+    <t>發表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>簡報</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -83,47 +132,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>草稿</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>關於</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>購物</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>發表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>草稿</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>簡報</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>簡報</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>商品</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主頁</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>排版</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -131,7 +140,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,8 +169,16 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,12 +188,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,21 +305,21 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -327,11 +338,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -630,16 +641,38 @@
   <dimension ref="A2:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="2" spans="1:18" ht="17.25" thickBot="1"/>
+    <row r="2" spans="1:18" ht="29.25" thickBot="1">
+      <c r="B2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+    </row>
     <row r="3" spans="1:18" ht="28.5" thickBot="1">
       <c r="A3" s="1"/>
       <c r="B3" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -648,8 +681,9 @@
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="12"/>
+      <c r="J3" s="17"/>
       <c r="K3" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
@@ -675,13 +709,14 @@
       <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="2"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="3" t="s">
         <v>1</v>
       </c>
@@ -697,39 +732,40 @@
       <c r="O4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" ht="27.75">
-      <c r="B5" s="5">
+      <c r="B5" s="6">
         <v>22</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <v>23</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <v>24</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="6">
         <v>25</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="6">
         <v>26</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="6">
         <v>27</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="6">
         <v>28</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>8</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="J5" s="17"/>
       <c r="K5" s="6">
         <v>22</v>
       </c>
@@ -745,67 +781,69 @@
       <c r="O5" s="6">
         <v>26</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="6">
         <v>27</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="6">
         <v>28</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="27.75">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="9"/>
+    </row>
+    <row r="7" spans="1:18" ht="27.75">
+      <c r="B7" s="6">
+        <v>29</v>
+      </c>
+      <c r="C7" s="6">
+        <v>30</v>
+      </c>
+      <c r="D7" s="6">
+        <v>31</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6">
+        <v>2</v>
+      </c>
+      <c r="G7" s="6">
+        <v>3</v>
+      </c>
+      <c r="H7" s="6">
+        <v>4</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="9"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="9"/>
-    </row>
-    <row r="7" spans="1:18" ht="27.75">
-      <c r="B7" s="5">
-        <v>29</v>
-      </c>
-      <c r="C7" s="5">
-        <v>30</v>
-      </c>
-      <c r="D7" s="5">
-        <v>31</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5">
-        <v>2</v>
-      </c>
-      <c r="G7" s="4">
-        <v>3</v>
-      </c>
-      <c r="H7" s="4">
-        <v>4</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="J7" s="17"/>
       <c r="K7" s="6">
         <v>29</v>
       </c>
@@ -821,45 +859,48 @@
       <c r="O7" s="6">
         <v>2</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="6">
         <v>3</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="6">
         <v>4</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="27.75">
-      <c r="B8" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
       <c r="I8" s="9"/>
-      <c r="K8" s="7" t="s">
+      <c r="J8" s="17"/>
+      <c r="K8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="O8" s="5"/>
+      <c r="P8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="4"/>
       <c r="R8" s="9"/>
     </row>
     <row r="9" spans="1:18" ht="27.75">
       <c r="B9" s="13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -868,8 +909,9 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
+      <c r="J9" s="17"/>
       <c r="K9" s="13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
@@ -880,30 +922,31 @@
       <c r="R9" s="15"/>
     </row>
     <row r="10" spans="1:18" ht="27.75">
-      <c r="B10" s="5">
+      <c r="B10" s="6">
         <v>5</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="6">
         <v>6</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="6">
         <v>7</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="6">
         <v>8</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="6">
         <v>9</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="6">
         <v>10</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="6">
         <v>11</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>10</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="J10" s="17"/>
       <c r="K10" s="6">
         <v>5</v>
       </c>
@@ -919,67 +962,67 @@
       <c r="O10" s="6">
         <v>9</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10" s="6">
         <v>10</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10" s="6">
         <v>11</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="27.75">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
       <c r="I11" s="9"/>
-      <c r="K11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="7"/>
-      <c r="M11" s="8" t="s">
+      <c r="J11" s="17"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
       <c r="R11" s="9"/>
     </row>
     <row r="12" spans="1:18" ht="27.75">
-      <c r="B12" s="5">
+      <c r="B12" s="6">
         <v>12</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="6">
         <v>13</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <v>14</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="6">
         <v>15</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="6">
         <v>16</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="6">
         <v>17</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="6">
         <v>18</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="J12" s="17"/>
       <c r="K12" s="6">
         <v>12</v>
       </c>
@@ -995,71 +1038,73 @@
       <c r="O12" s="6">
         <v>16</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12" s="6">
         <v>17</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="Q12" s="6">
         <v>18</v>
       </c>
       <c r="R12" s="9" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="27.75">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="I13" s="9"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O13" s="7" t="s">
+      <c r="J13" s="17"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" s="4"/>
+      <c r="P13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8" t="s">
+      <c r="Q13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R13" s="9"/>
+    </row>
+    <row r="14" spans="1:18" ht="27.75">
+      <c r="B14" s="6">
+        <v>19</v>
+      </c>
+      <c r="C14" s="6">
+        <v>20</v>
+      </c>
+      <c r="D14" s="6">
+        <v>21</v>
+      </c>
+      <c r="E14" s="6">
+        <v>22</v>
+      </c>
+      <c r="F14" s="6">
+        <v>23</v>
+      </c>
+      <c r="G14" s="6">
         <v>24</v>
       </c>
-      <c r="R13" s="9"/>
-    </row>
-    <row r="14" spans="1:18" ht="27.75">
-      <c r="B14" s="5">
-        <v>19</v>
-      </c>
-      <c r="C14" s="5">
-        <v>20</v>
-      </c>
-      <c r="D14" s="5">
-        <v>21</v>
-      </c>
-      <c r="E14" s="5">
-        <v>22</v>
-      </c>
-      <c r="F14" s="5">
-        <v>23</v>
-      </c>
-      <c r="G14" s="4">
-        <v>24</v>
-      </c>
-      <c r="H14" s="4">
+      <c r="H14" s="6">
         <v>25</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>7</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="J14" s="17"/>
       <c r="K14" s="6">
         <v>19</v>
       </c>
@@ -1075,40 +1120,50 @@
       <c r="O14" s="6">
         <v>23</v>
       </c>
-      <c r="P14" s="4">
+      <c r="P14" s="6">
         <v>24</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="Q14" s="6">
         <v>25</v>
       </c>
       <c r="R14" s="9" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="27.75">
-      <c r="B15" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="B15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
       <c r="I15" s="9"/>
-      <c r="K15" s="17" t="s">
-        <v>21</v>
+      <c r="J15" s="17"/>
+      <c r="K15" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
       <c r="R15" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="R12:R13"/>
+    <mergeCell ref="R14:R15"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="R10:R11"/>
     <mergeCell ref="I12:I13"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="B3:I3"/>
@@ -1116,13 +1171,6 @@
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="I10:I11"/>
-    <mergeCell ref="R12:R13"/>
-    <mergeCell ref="R14:R15"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="K9:R9"/>
-    <mergeCell ref="R10:R11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>